<commit_message>
cocktail page displays donor excel info
</commit_message>
<xml_diff>
--- a/src/data/donations.xlsx
+++ b/src/data/donations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bramschork/Documents/cocktails/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90606EEB-BAC0-A943-8A80-4524954C2013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ADBF1D-C19C-FD4C-B7A4-EEC5216CB1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17220" xr2:uid="{697828C2-5AED-E048-8AD6-CBFEB80D738D}"/>
   </bookViews>
@@ -473,7 +473,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>